<commit_message>
feat:update new doll machine and level bug
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/DollMachine_娃娃机.xlsx
+++ b/pet-simulator/Excel/DollMachine_娃娃机.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaWorldSaved\Saved\MetaWorld\Project\Edit\Dragonverse\pet-simulator\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC097D6-027A-4EEC-ACEA-7FC7578ECC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>int</t>
   </si>
@@ -145,21 +141,50 @@
   </si>
   <si>
     <t>21|22|23|24|25|26</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>18|18|18|18|14|14</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1A2FBB46</t>
+  </si>
+  <si>
+    <t>2CD6E055</t>
+  </si>
+  <si>
+    <t>1373C93C</t>
+  </si>
+  <si>
+    <t>128B337C</t>
+  </si>
+  <si>
+    <t>0F9E4AE8</t>
+  </si>
+  <si>
+    <t>0086F8FB|3D5F0855|3B0BEC6C|28C7C1E5</t>
+  </si>
+  <si>
+    <t>13EE55E0</t>
+  </si>
+  <si>
+    <t>3E914E69|25D1C5F5</t>
+  </si>
+  <si>
+    <t>38B58E75</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * \-??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -169,50 +194,372 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -220,11 +567,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -234,174 +823,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -412,7 +931,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -440,40 +959,154 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
+          <color theme="4" tint="0.399975585192419"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -731,19 +1364,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="13.125" customWidth="1"/>
     <col min="3" max="3" width="15.375" style="2" customWidth="1"/>
@@ -753,12 +1386,12 @@
     <col min="7" max="7" width="28.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="18.125" customWidth="1"/>
     <col min="9" max="9" width="19.625" customWidth="1"/>
-    <col min="11" max="11" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.625" customWidth="1"/>
+    <col min="12" max="12" width="16.125" customWidth="1"/>
     <col min="1022" max="1022" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -796,7 +1429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -834,7 +1467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" s="1" customFormat="1" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -872,7 +1505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" s="1" customFormat="1" spans="1:12">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -886,7 +1519,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1</v>
       </c>
@@ -917,36 +1550,69 @@
       <c r="J5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="9:12">
       <c r="I7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="9:12">
       <c r="I8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="9:12">
       <c r="I9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>